<commit_message>
Leitura dos arquivos csv
</commit_message>
<xml_diff>
--- a/config/eda.xlsx
+++ b/config/eda.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/72364bdb7555e539/Documentos/GitHub/eda-o-matic/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{8558213C-73DF-456B-87B3-94B50D5359AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D60F85E-4EBA-4884-AB7F-A5055B7675AB}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{8558213C-73DF-456B-87B3-94B50D5359AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7D76558-1F9F-4D6E-B2B7-A21E66CF652C}"/>
   <bookViews>
-    <workbookView xWindow="29940" yWindow="1140" windowWidth="22860" windowHeight="10215" xr2:uid="{3AA627A5-71EE-4E50-888B-47FA87E80BB2}"/>
+    <workbookView xWindow="34020" yWindow="2010" windowWidth="18420" windowHeight="10215" activeTab="1" xr2:uid="{3AA627A5-71EE-4E50-888B-47FA87E80BB2}"/>
   </bookViews>
   <sheets>
     <sheet name="validations" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="291">
   <si>
     <t>df['col'].str.strip().eq('')</t>
   </si>
@@ -932,6 +932,33 @@
   </si>
   <si>
     <t>routine</t>
+  </si>
+  <si>
+    <t>ses_seguros.csv</t>
+  </si>
+  <si>
+    <t>ses_seguros</t>
+  </si>
+  <si>
+    <t>coenti</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>ses_cias</t>
+  </si>
+  <si>
+    <t>ses_cias.csv</t>
+  </si>
+  <si>
+    <t>ses_ramos</t>
+  </si>
+  <si>
+    <t>coramo</t>
+  </si>
+  <si>
+    <t>ses_ramos.csv</t>
   </si>
 </sst>
 </file>
@@ -1131,7 +1158,21 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="5">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1465,7 +1506,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5128729E-CAE0-4D53-8104-6E53847E91FB}">
   <dimension ref="A1:J69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
@@ -3330,7 +3371,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H2:J60">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula>"undefined"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3348,14 +3389,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8E3DCC3-C2E9-497C-93AD-C6BE814847A7}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
+    <col min="1" max="1" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.81640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.90625" bestFit="1" customWidth="1"/>
@@ -3411,44 +3452,124 @@
       </c>
     </row>
     <row r="2" spans="1:14">
+      <c r="A2" t="s">
+        <v>282</v>
+      </c>
+      <c r="B2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C2" t="s">
+        <v>284</v>
+      </c>
       <c r="D2" t="s">
-        <v>79</v>
+        <v>277</v>
       </c>
       <c r="E2" t="s">
-        <v>79</v>
+        <v>285</v>
       </c>
       <c r="F2" t="s">
-        <v>79</v>
+        <v>270</v>
       </c>
       <c r="G2" t="s">
-        <v>79</v>
+        <v>271</v>
       </c>
       <c r="H2" t="s">
-        <v>79</v>
+        <v>271</v>
+      </c>
+      <c r="I2" t="s">
+        <v>286</v>
       </c>
       <c r="N2" t="s">
-        <v>79</v>
+        <v>271</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" t="s">
+        <v>287</v>
+      </c>
+      <c r="B3" t="s">
+        <v>286</v>
+      </c>
+      <c r="C3" t="s">
+        <v>284</v>
+      </c>
+      <c r="D3" t="s">
+        <v>277</v>
+      </c>
+      <c r="E3" t="s">
+        <v>285</v>
+      </c>
+      <c r="F3" t="s">
+        <v>270</v>
+      </c>
+      <c r="G3" t="s">
+        <v>271</v>
+      </c>
+      <c r="H3" t="s">
+        <v>270</v>
+      </c>
+      <c r="N3" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" t="s">
+        <v>290</v>
+      </c>
+      <c r="B4" t="s">
+        <v>288</v>
+      </c>
+      <c r="C4" t="s">
+        <v>289</v>
+      </c>
+      <c r="D4" t="s">
+        <v>277</v>
+      </c>
+      <c r="E4" t="s">
+        <v>285</v>
+      </c>
+      <c r="F4" t="s">
+        <v>270</v>
+      </c>
+      <c r="G4" t="s">
+        <v>271</v>
+      </c>
+      <c r="H4" t="s">
+        <v>270</v>
+      </c>
+      <c r="N4" t="s">
+        <v>271</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:H2">
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+  <conditionalFormatting sqref="D2:I2">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
       <formula>"undefined"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2">
+  <conditionalFormatting sqref="N2:N23">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>"undefined"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:I3">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"undefined"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4:I23">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"undefined"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{1BD25EFA-FFA7-4AE3-84CE-F90A862E844B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D23" xr:uid="{1BD25EFA-FFA7-4AE3-84CE-F90A862E844B}">
       <formula1>"undefined,number,text,data"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{7BF78B2D-6704-42D1-8A77-BCB96BCA9F64}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E23" xr:uid="{7BF78B2D-6704-42D1-8A77-BCB96BCA9F64}">
       <formula1>"undefined,integer,decimal"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2 F2:H2" xr:uid="{A381429F-140A-4013-AD16-6E46B19FCE63}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N23 F2:H23" xr:uid="{A381429F-140A-4013-AD16-6E46B19FCE63}">
       <formula1>"undefined,yes,no"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Mecanismo de característica x validação
</commit_message>
<xml_diff>
--- a/config/eda.xlsx
+++ b/config/eda.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/72364bdb7555e539/Documentos/GitHub/eda-o-matic/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="8_{8558213C-73DF-456B-87B3-94B50D5359AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7989806B-6475-40F1-8870-083A715D1813}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="8_{8558213C-73DF-456B-87B3-94B50D5359AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F92F53C8-C1C9-4121-B1FC-15E2764DF837}"/>
   <bookViews>
-    <workbookView xWindow="29520" yWindow="3810" windowWidth="24225" windowHeight="10215" activeTab="1" xr2:uid="{3AA627A5-71EE-4E50-888B-47FA87E80BB2}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3AA627A5-71EE-4E50-888B-47FA87E80BB2}"/>
   </bookViews>
   <sheets>
     <sheet name="validations" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="308">
   <si>
     <t>df['col'].str.strip().eq('')</t>
   </si>
@@ -325,9 +325,6 @@
     <t>category</t>
   </si>
   <si>
-    <t xml:space="preserve">test </t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
@@ -667,9 +664,6 @@
     <t xml:space="preserve">null_empty  </t>
   </si>
   <si>
-    <t xml:space="preserve">zero_values  </t>
-  </si>
-  <si>
     <t xml:space="preserve">constant_values  </t>
   </si>
   <si>
@@ -974,6 +968,48 @@
   </si>
   <si>
     <t>xxx</t>
+  </si>
+  <si>
+    <t>number, range</t>
+  </si>
+  <si>
+    <t>number, decimal</t>
+  </si>
+  <si>
+    <t>text, format</t>
+  </si>
+  <si>
+    <t>values_list</t>
+  </si>
+  <si>
+    <t>Verify a list of valid values</t>
+  </si>
+  <si>
+    <t>valuies list</t>
+  </si>
+  <si>
+    <t>check_values_list</t>
+  </si>
+  <si>
+    <t>zero, negative</t>
+  </si>
+  <si>
+    <t>check_zero_negative</t>
+  </si>
+  <si>
+    <t>zero_negative_vaues</t>
+  </si>
+  <si>
+    <t>zero</t>
+  </si>
+  <si>
+    <t>negative</t>
+  </si>
+  <si>
+    <t>nulo</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -1120,7 +1156,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1169,10 +1205,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1511,18 +1548,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5128729E-CAE0-4D53-8104-6E53847E91FB}">
-  <dimension ref="A1:K69"/>
+  <dimension ref="A1:K70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomLeft" activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="36.36328125" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="26.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33" style="1" customWidth="1"/>
     <col min="5" max="5" width="60.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="38.1796875" style="1" customWidth="1"/>
@@ -1536,34 +1573,34 @@
   <sheetData>
     <row r="1" spans="1:11" s="13" customFormat="1">
       <c r="A1" s="10" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>78</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D1" s="12" t="s">
+        <v>307</v>
+      </c>
+      <c r="E1" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="F1" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="F1" s="12" t="s">
-        <v>81</v>
-      </c>
       <c r="G1" s="12" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="K1" s="12" t="s">
         <v>76</v>
@@ -1571,153 +1608,159 @@
     </row>
     <row r="2" spans="1:11" s="19" customFormat="1">
       <c r="A2" s="18" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>64</v>
       </c>
       <c r="D2" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="E2" t="s">
         <v>262</v>
-      </c>
-      <c r="E2" t="s">
-        <v>264</v>
       </c>
       <c r="F2" s="18"/>
       <c r="G2" s="18"/>
       <c r="H2" s="18" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="I2" s="20" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="J2" s="20" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="K2" s="22" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="19" customFormat="1">
       <c r="A3" s="18" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>64</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F3" s="18"/>
       <c r="G3" s="18"/>
       <c r="H3" s="18" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="I3" s="20" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="J3" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="K3" s="20" t="s">
-        <v>268</v>
+        <v>81</v>
+      </c>
+      <c r="K3" s="22" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>83</v>
+        <v>291</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>306</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>82</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>292</v>
+      <c r="G4" s="21" t="s">
+        <v>290</v>
       </c>
       <c r="H4" s="18" t="s">
-        <v>290</v>
-      </c>
-      <c r="I4" s="23" t="s">
-        <v>268</v>
-      </c>
-      <c r="J4" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="K4" s="20" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+        <v>288</v>
+      </c>
+      <c r="I4" s="22" t="s">
+        <v>266</v>
+      </c>
+      <c r="J4" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="K4" s="22" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="13" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>193</v>
+        <v>303</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>274</v>
+        <v>301</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
+      <c r="G5" s="21" t="s">
+        <v>290</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>302</v>
+      </c>
       <c r="I5" s="20" t="s">
         <v>77</v>
       </c>
       <c r="J5" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="K5" s="20" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="K5" s="22" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="12" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>194</v>
+        <v>297</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>274</v>
+        <v>291</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>74</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>85</v>
+        <v>299</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
+        <v>298</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>300</v>
+      </c>
       <c r="I6" s="20" t="s">
         <v>77</v>
       </c>
@@ -1725,30 +1768,30 @@
         <v>77</v>
       </c>
       <c r="K6" s="20" t="s">
-        <v>77</v>
+        <v>265</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>86</v>
+        <v>272</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
+        <v>136</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
       <c r="I7" s="20" t="s">
         <v>77</v>
       </c>
@@ -1761,25 +1804,25 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>274</v>
+        <v>294</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
+        <v>137</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
       <c r="I8" s="20" t="s">
         <v>77</v>
       </c>
@@ -1792,22 +1835,22 @@
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>274</v>
+        <v>295</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
@@ -1823,25 +1866,25 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
+        <v>139</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
       <c r="I10" s="20" t="s">
         <v>77</v>
       </c>
@@ -1854,25 +1897,25 @@
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
+        <v>140</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
       <c r="I11" s="20" t="s">
         <v>77</v>
       </c>
@@ -1885,25 +1928,25 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12" s="4"/>
-      <c r="H12" s="21"/>
+      <c r="H12" s="4"/>
       <c r="I12" s="20" t="s">
         <v>77</v>
       </c>
@@ -1916,25 +1959,25 @@
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
+      <c r="H13" s="21"/>
       <c r="I13" s="20" t="s">
         <v>77</v>
       </c>
@@ -1947,22 +1990,22 @@
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
@@ -1978,22 +2021,22 @@
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>275</v>
+        <v>296</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
@@ -2009,22 +2052,22 @@
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="2" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
@@ -2040,22 +2083,22 @@
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
@@ -2071,22 +2114,22 @@
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
@@ -2102,22 +2145,22 @@
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
@@ -2133,22 +2176,22 @@
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
@@ -2164,22 +2207,22 @@
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
@@ -2195,22 +2238,22 @@
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
@@ -2226,25 +2269,25 @@
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>251</v>
+        <v>291</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
+        <v>152</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
       <c r="I23" s="20" t="s">
         <v>77</v>
       </c>
@@ -2257,25 +2300,25 @@
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
+        <v>153</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
       <c r="I24" s="20" t="s">
         <v>77</v>
       </c>
@@ -2288,22 +2331,22 @@
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
@@ -2319,23 +2362,25 @@
     </row>
     <row r="26" spans="1:11">
       <c r="A26" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>16</v>
+        <v>103</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
+        <v>155</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
       <c r="I26" s="20" t="s">
         <v>77</v>
       </c>
@@ -2348,25 +2393,23 @@
     </row>
     <row r="27" spans="1:11">
       <c r="A27" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>105</v>
+        <v>16</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
+        <v>156</v>
+      </c>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
       <c r="I27" s="20" t="s">
         <v>77</v>
       </c>
@@ -2379,22 +2422,22 @@
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
@@ -2410,22 +2453,22 @@
     </row>
     <row r="29" spans="1:11">
       <c r="A29" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
@@ -2440,23 +2483,23 @@
       </c>
     </row>
     <row r="30" spans="1:11">
-      <c r="A30" s="1" t="s">
-        <v>218</v>
+      <c r="A30" s="2" t="s">
+        <v>215</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>26</v>
+        <v>106</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G30" s="7"/>
       <c r="H30" s="7"/>
@@ -2472,22 +2515,22 @@
     </row>
     <row r="31" spans="1:11">
       <c r="A31" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>108</v>
+        <v>26</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G31" s="7"/>
       <c r="H31" s="7"/>
@@ -2503,22 +2546,22 @@
     </row>
     <row r="32" spans="1:11">
       <c r="A32" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G32" s="7"/>
       <c r="H32" s="7"/>
@@ -2534,22 +2577,22 @@
     </row>
     <row r="33" spans="1:11">
       <c r="A33" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
@@ -2565,22 +2608,22 @@
     </row>
     <row r="34" spans="1:11">
       <c r="A34" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G34" s="7"/>
       <c r="H34" s="7"/>
@@ -2596,22 +2639,22 @@
     </row>
     <row r="35" spans="1:11">
       <c r="A35" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G35" s="7"/>
       <c r="H35" s="7"/>
@@ -2625,24 +2668,24 @@
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="16.5" customHeight="1">
+    <row r="36" spans="1:11">
       <c r="A36" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G36" s="7"/>
       <c r="H36" s="7"/>
@@ -2656,24 +2699,24 @@
         <v>77</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" ht="16.5" customHeight="1">
       <c r="A37" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>34</v>
+        <v>112</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G37" s="7"/>
       <c r="H37" s="7"/>
@@ -2689,22 +2732,22 @@
     </row>
     <row r="38" spans="1:11">
       <c r="A38" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>114</v>
+        <v>34</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G38" s="7"/>
       <c r="H38" s="7"/>
@@ -2720,22 +2763,22 @@
     </row>
     <row r="39" spans="1:11">
       <c r="A39" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
@@ -2751,22 +2794,22 @@
     </row>
     <row r="40" spans="1:11">
       <c r="A40" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>38</v>
+        <v>114</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G40" s="7"/>
       <c r="H40" s="7"/>
@@ -2782,22 +2825,22 @@
     </row>
     <row r="41" spans="1:11">
       <c r="A41" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G41" s="7"/>
       <c r="H41" s="7"/>
@@ -2813,25 +2856,25 @@
     </row>
     <row r="42" spans="1:11">
       <c r="A42" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>116</v>
+        <v>40</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="G42" s="6"/>
-      <c r="H42" s="6"/>
+        <v>171</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7"/>
       <c r="I42" s="20" t="s">
         <v>77</v>
       </c>
@@ -2844,25 +2887,25 @@
     </row>
     <row r="43" spans="1:11">
       <c r="A43" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="G43" s="7"/>
-      <c r="H43" s="7"/>
+        <v>172</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
       <c r="I43" s="20" t="s">
         <v>77</v>
       </c>
@@ -2875,25 +2918,25 @@
     </row>
     <row r="44" spans="1:11">
       <c r="A44" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="G44" s="6"/>
-      <c r="H44" s="6"/>
+        <v>173</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
       <c r="I44" s="20" t="s">
         <v>77</v>
       </c>
@@ -2906,25 +2949,25 @@
     </row>
     <row r="45" spans="1:11">
       <c r="A45" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="G45" s="7"/>
-      <c r="H45" s="7"/>
+        <v>174</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
       <c r="I45" s="20" t="s">
         <v>77</v>
       </c>
@@ -2937,22 +2980,22 @@
     </row>
     <row r="46" spans="1:11">
       <c r="A46" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>50</v>
+        <v>274</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G46" s="7"/>
       <c r="H46" s="7"/>
@@ -2968,22 +3011,22 @@
     </row>
     <row r="47" spans="1:11">
       <c r="A47" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>50</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G47" s="7"/>
       <c r="H47" s="7"/>
@@ -2997,24 +3040,24 @@
         <v>77</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="25">
+    <row r="48" spans="1:11">
       <c r="A48" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>50</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G48" s="7"/>
       <c r="H48" s="7"/>
@@ -3028,24 +3071,24 @@
         <v>77</v>
       </c>
     </row>
-    <row r="49" spans="1:11">
+    <row r="49" spans="1:11" ht="25">
       <c r="A49" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>50</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G49" s="7"/>
       <c r="H49" s="7"/>
@@ -3061,22 +3104,22 @@
     </row>
     <row r="50" spans="1:11">
       <c r="A50" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>50</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G50" s="7"/>
       <c r="H50" s="7"/>
@@ -3090,24 +3133,24 @@
         <v>77</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="25">
+    <row r="51" spans="1:11">
       <c r="A51" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>45</v>
+        <v>254</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>50</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G51" s="7"/>
       <c r="H51" s="7"/>
@@ -3121,24 +3164,24 @@
         <v>77</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="23.5" customHeight="1">
+    <row r="52" spans="1:11" ht="25">
       <c r="A52" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G52" s="7"/>
       <c r="H52" s="7"/>
@@ -3152,9 +3195,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="53" spans="1:11">
+    <row r="53" spans="1:11" ht="23.5" customHeight="1">
       <c r="A53" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>45</v>
@@ -3163,13 +3206,13 @@
         <v>53</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G53" s="7"/>
       <c r="H53" s="7"/>
@@ -3185,22 +3228,22 @@
     </row>
     <row r="54" spans="1:11">
       <c r="A54" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>257</v>
+        <v>45</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>53</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G54" s="7"/>
       <c r="H54" s="7"/>
@@ -3216,22 +3259,22 @@
     </row>
     <row r="55" spans="1:11">
       <c r="A55" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>53</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G55" s="7"/>
       <c r="H55" s="7"/>
@@ -3245,24 +3288,24 @@
         <v>77</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="25">
+    <row r="56" spans="1:11">
       <c r="A56" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>53</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G56" s="7"/>
       <c r="H56" s="7"/>
@@ -3278,22 +3321,22 @@
     </row>
     <row r="57" spans="1:11" ht="25">
       <c r="A57" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>53</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G57" s="7"/>
       <c r="H57" s="7"/>
@@ -3307,24 +3350,24 @@
         <v>77</v>
       </c>
     </row>
-    <row r="58" spans="1:11">
+    <row r="58" spans="1:11" ht="25">
       <c r="A58" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>53</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G58" s="7"/>
       <c r="H58" s="7"/>
@@ -3338,27 +3381,27 @@
         <v>77</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="29">
+    <row r="59" spans="1:11">
       <c r="A59" s="1" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>53</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="F59" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="G59" s="6"/>
-      <c r="H59" s="6"/>
+        <v>188</v>
+      </c>
+      <c r="F59" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="G59" s="7"/>
+      <c r="H59" s="7"/>
       <c r="I59" s="20" t="s">
         <v>77</v>
       </c>
@@ -3369,27 +3412,27 @@
         <v>77</v>
       </c>
     </row>
-    <row r="60" spans="1:11">
+    <row r="60" spans="1:11" ht="29">
       <c r="A60" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>53</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="F60" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="G60" s="7"/>
-      <c r="H60" s="7"/>
+        <v>189</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G60" s="6"/>
+      <c r="H60" s="6"/>
       <c r="I60" s="20" t="s">
         <v>77</v>
       </c>
@@ -3401,64 +3444,95 @@
       </c>
     </row>
     <row r="61" spans="1:11">
+      <c r="A61" s="1" t="s">
+        <v>246</v>
+      </c>
       <c r="B61" s="1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>53</v>
       </c>
+      <c r="D61" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="F61" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="G61" s="7"/>
+      <c r="H61" s="7"/>
+      <c r="I61" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="J61" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="K61" s="20" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="62" spans="1:11">
       <c r="B62" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="63" spans="1:11">
       <c r="B63" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="64" spans="1:11">
       <c r="B64" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="65" spans="2:2">
       <c r="B65" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="66" spans="2:2">
       <c r="B66" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="67" spans="2:2">
       <c r="B67" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="68" spans="2:2">
       <c r="B68" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="69" spans="2:2">
       <c r="B69" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2">
+      <c r="B70" s="1" t="s">
+        <v>258</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I2:K60">
+  <conditionalFormatting sqref="I2:K61">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"undefined"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K60 I2:I60" xr:uid="{E4DF7DBE-233E-4CAB-B72C-331851F0FA04}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K61 I2:I61" xr:uid="{E4DF7DBE-233E-4CAB-B72C-331851F0FA04}">
       <formula1>"undefined,yes,no"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J60" xr:uid="{27BB500F-5D24-420A-87D6-C1F235E36EA2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J61" xr:uid="{27BB500F-5D24-420A-87D6-C1F235E36EA2}">
       <formula1>"undefined,check,info"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3469,10 +3543,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8E3DCC3-C2E9-497C-93AD-C6BE814847A7}">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3482,14 +3556,15 @@
     <col min="4" max="4" width="9.81640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.453125" customWidth="1"/>
-    <col min="12" max="12" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.90625" customWidth="1"/>
+    <col min="9" max="10" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.453125" customWidth="1"/>
+    <col min="14" max="14" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:16">
       <c r="A1" s="9" t="s">
         <v>64</v>
       </c>
@@ -3509,169 +3584,200 @@
         <v>69</v>
       </c>
       <c r="G1" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="I1" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="K1" s="8" t="s">
-        <v>294</v>
-      </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="N1" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="O1" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="P1" s="8" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
+        <v>277</v>
+      </c>
+      <c r="B2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C2" t="s">
         <v>279</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
+        <v>272</v>
+      </c>
+      <c r="E2" t="s">
         <v>280</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
+        <v>265</v>
+      </c>
+      <c r="G2" t="s">
+        <v>265</v>
+      </c>
+      <c r="H2" t="s">
+        <v>265</v>
+      </c>
+      <c r="I2" t="s">
+        <v>266</v>
+      </c>
+      <c r="J2" t="s">
+        <v>266</v>
+      </c>
+      <c r="K2" t="s">
         <v>281</v>
       </c>
-      <c r="D2" t="s">
-        <v>274</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="P2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" t="s">
         <v>282</v>
       </c>
-      <c r="F2" t="s">
-        <v>267</v>
-      </c>
-      <c r="G2" t="s">
-        <v>268</v>
-      </c>
-      <c r="H2" t="s">
-        <v>268</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="B3" t="s">
+        <v>281</v>
+      </c>
+      <c r="C3" t="s">
+        <v>279</v>
+      </c>
+      <c r="D3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E3" t="s">
+        <v>280</v>
+      </c>
+      <c r="F3" t="s">
+        <v>265</v>
+      </c>
+      <c r="G3" t="s">
+        <v>265</v>
+      </c>
+      <c r="H3" t="s">
+        <v>265</v>
+      </c>
+      <c r="I3" t="s">
+        <v>266</v>
+      </c>
+      <c r="J3" t="s">
+        <v>265</v>
+      </c>
+      <c r="N3">
+        <v>123</v>
+      </c>
+      <c r="P3" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" t="s">
+        <v>285</v>
+      </c>
+      <c r="B4" t="s">
         <v>283</v>
       </c>
-      <c r="N2" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3" t="s">
+      <c r="C4" t="s">
         <v>284</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E4" t="s">
+        <v>280</v>
+      </c>
+      <c r="F4" t="s">
+        <v>265</v>
+      </c>
+      <c r="G4" t="s">
+        <v>265</v>
+      </c>
+      <c r="H4" t="s">
+        <v>265</v>
+      </c>
+      <c r="I4" t="s">
+        <v>266</v>
+      </c>
+      <c r="J4" t="s">
+        <v>265</v>
+      </c>
+      <c r="L4" t="s">
+        <v>293</v>
+      </c>
+      <c r="M4">
+        <v>1.2</v>
+      </c>
+      <c r="P4" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B5" t="s">
         <v>283</v>
       </c>
-      <c r="C3" t="s">
-        <v>281</v>
-      </c>
-      <c r="D3" t="s">
-        <v>274</v>
-      </c>
-      <c r="E3" t="s">
-        <v>282</v>
-      </c>
-      <c r="F3" t="s">
-        <v>267</v>
-      </c>
-      <c r="G3" t="s">
-        <v>268</v>
-      </c>
-      <c r="H3" t="s">
-        <v>267</v>
-      </c>
-      <c r="L3">
-        <v>123</v>
-      </c>
-      <c r="N3" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4" t="s">
-        <v>287</v>
-      </c>
-      <c r="B4" t="s">
-        <v>285</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>286</v>
       </c>
-      <c r="D4" t="s">
-        <v>274</v>
-      </c>
-      <c r="E4" t="s">
-        <v>282</v>
-      </c>
-      <c r="F4" t="s">
-        <v>267</v>
-      </c>
-      <c r="G4" t="s">
-        <v>268</v>
-      </c>
-      <c r="H4" t="s">
-        <v>267</v>
-      </c>
-      <c r="J4" t="s">
-        <v>295</v>
-      </c>
-      <c r="K4">
-        <v>1.2</v>
-      </c>
-      <c r="N4" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="A5" t="s">
-        <v>287</v>
-      </c>
-      <c r="B5" t="s">
-        <v>285</v>
-      </c>
-      <c r="C5" t="s">
-        <v>288</v>
-      </c>
       <c r="D5" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E5" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F5" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="G5" t="s">
-        <v>268</v>
-      </c>
-      <c r="H5" t="s">
-        <v>267</v>
-      </c>
-      <c r="L5" s="1"/>
-      <c r="N5" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
+        <v>265</v>
+      </c>
+      <c r="H5" s="23" t="s">
+        <v>265</v>
+      </c>
+      <c r="I5" t="s">
+        <v>266</v>
+      </c>
+      <c r="J5" t="s">
+        <v>265</v>
+      </c>
+      <c r="N5" s="1"/>
+      <c r="P5" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
       <c r="E8" s="14"/>
+      <c r="I8" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:I23 J4">
+  <conditionalFormatting sqref="D2:K23 L4">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"undefined"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N23">
+  <conditionalFormatting sqref="P2:P23">
     <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"undefined"</formula>
     </cfRule>
@@ -3683,7 +3789,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E23" xr:uid="{7BF78B2D-6704-42D1-8A77-BCB96BCA9F64}">
       <formula1>"undefined,integer,decimal"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:H23 N2:N23" xr:uid="{A381429F-140A-4013-AD16-6E46B19FCE63}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P23 F2:J23" xr:uid="{A381429F-140A-4013-AD16-6E46B19FCE63}">
       <formula1>"undefined,yes,no"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Correção de bugs diversos nas novas regras
</commit_message>
<xml_diff>
--- a/config/eda.xlsx
+++ b/config/eda.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/72364bdb7555e539/Documentos/GitHub/eda-o-matic/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="85" documentId="8_{8558213C-73DF-456B-87B3-94B50D5359AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4AB7050E-EF7E-4CA2-8F75-5DA8638CA1EA}"/>
+  <xr:revisionPtr revIDLastSave="87" documentId="8_{8558213C-73DF-456B-87B3-94B50D5359AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00A8AC82-8944-4F30-A845-97539C112EE4}"/>
   <bookViews>
     <workbookView xWindow="30630" yWindow="1575" windowWidth="24225" windowHeight="13440" xr2:uid="{3AA627A5-71EE-4E50-888B-47FA87E80BB2}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="301">
   <si>
     <t>df['col'].str.strip().eq('')</t>
   </si>
@@ -79,9 +79,6 @@
     <t>df['col'].astype(str).str.split('.').str[1].str.len()</t>
   </si>
   <si>
-    <t>df['col'].dtype</t>
-  </si>
-  <si>
     <t xml:space="preserve">Exemplo: Total da venda = -100 </t>
   </si>
   <si>
@@ -274,9 +271,6 @@
     <t>Precision / decimal places</t>
   </si>
   <si>
-    <t>Incorrect numeric type</t>
-  </si>
-  <si>
     <t>Statistical description of values</t>
   </si>
   <si>
@@ -427,9 +421,6 @@
     <t>May indicate formatting inconsistency.</t>
   </si>
   <si>
-    <t>Numeric values stored as text.</t>
-  </si>
-  <si>
     <t>Mean, median, standard deviation, etc.</t>
   </si>
   <si>
@@ -587,9 +578,6 @@
   </si>
   <si>
     <t xml:space="preserve">decimal_precision  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">invalid_numeric_type  </t>
   </si>
   <si>
     <t xml:space="preserve">statistical_summary  </t>
@@ -973,10 +961,10 @@
     <t>check_valid_range</t>
   </si>
   <si>
-    <t>de 1111 a 9999</t>
-  </si>
-  <si>
     <t>decimal</t>
+  </si>
+  <si>
+    <t>de 1111 a 99999</t>
   </si>
 </sst>
 </file>
@@ -1135,7 +1123,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1196,6 +1184,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -1237,7 +1231,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1332,11 +1326,18 @@
     <xf numFmtId="0" fontId="11" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1674,11 +1675,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5128729E-CAE0-4D53-8104-6E53847E91FB}">
-  <dimension ref="A1:J60"/>
+  <dimension ref="A1:J59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9:F9"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="36.36328125" defaultRowHeight="14.5"/>
@@ -1698,155 +1699,155 @@
   <sheetData>
     <row r="1" spans="1:10" s="5" customFormat="1" ht="18.5">
       <c r="A1" s="25" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B1" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>258</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>275</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>281</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>259</v>
+      </c>
+      <c r="G1" s="27" t="s">
+        <v>277</v>
+      </c>
+      <c r="H1" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="26" t="s">
-        <v>262</v>
-      </c>
-      <c r="D1" s="27" t="s">
-        <v>279</v>
-      </c>
-      <c r="E1" s="27" t="s">
-        <v>285</v>
-      </c>
-      <c r="F1" s="27" t="s">
-        <v>263</v>
-      </c>
-      <c r="G1" s="27" t="s">
-        <v>281</v>
-      </c>
-      <c r="H1" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="17" t="s">
         <v>75</v>
-      </c>
-      <c r="J1" s="17" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="13" customFormat="1" ht="18.5">
       <c r="A2" s="28" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D2" s="28" t="s">
+        <v>245</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>279</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>278</v>
+      </c>
+      <c r="G2" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="H2" s="34" t="s">
         <v>249</v>
       </c>
-      <c r="E2" s="28" t="s">
-        <v>283</v>
-      </c>
-      <c r="F2" s="28" t="s">
-        <v>282</v>
-      </c>
-      <c r="G2" s="34" t="s">
-        <v>254</v>
-      </c>
-      <c r="H2" s="34" t="s">
-        <v>253</v>
-      </c>
       <c r="I2" s="18" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="J2" s="14"/>
     </row>
     <row r="3" spans="1:10" s="13" customFormat="1" ht="18.5">
       <c r="A3" s="28" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="E3" s="28" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="F3" s="28" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="G3" s="34" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H3" s="34" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="I3" s="19" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="J3" s="14"/>
     </row>
     <row r="4" spans="1:10" s="8" customFormat="1" ht="18.5">
       <c r="A4" s="30" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E4" s="31" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="F4" s="28" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="G4" s="35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H4" s="35" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="I4" s="20" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J4" s="15" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="18.5">
       <c r="A5" s="30" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="F5" s="30" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="G5" s="35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H5" s="35" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="I5" s="21" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="J5" s="22" t="s">
         <v>3</v>
@@ -1854,95 +1855,95 @@
     </row>
     <row r="6" spans="1:10" ht="18.5">
       <c r="A6" s="30" t="s">
+        <v>290</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>271</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>292</v>
+      </c>
+      <c r="D6" s="30" t="s">
         <v>294</v>
       </c>
-      <c r="B6" s="30" t="s">
-        <v>275</v>
-      </c>
-      <c r="C6" s="33" t="s">
+      <c r="E6" s="30" t="s">
+        <v>282</v>
+      </c>
+      <c r="F6" s="30" t="s">
         <v>296</v>
       </c>
-      <c r="D6" s="30" t="s">
-        <v>298</v>
-      </c>
-      <c r="E6" s="30" t="s">
-        <v>286</v>
-      </c>
-      <c r="F6" s="30" t="s">
-        <v>300</v>
-      </c>
       <c r="G6" s="35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H6" s="35" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="I6" s="21" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J6" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="18.5">
       <c r="A7" s="30" t="s">
+        <v>291</v>
+      </c>
+      <c r="B7" s="30" t="s">
+        <v>271</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>293</v>
+      </c>
+      <c r="D7" s="30" t="s">
         <v>295</v>
       </c>
-      <c r="B7" s="30" t="s">
-        <v>275</v>
-      </c>
-      <c r="C7" s="33" t="s">
+      <c r="E7" s="30" t="s">
+        <v>282</v>
+      </c>
+      <c r="F7" s="30" t="s">
         <v>297</v>
       </c>
-      <c r="D7" s="30" t="s">
-        <v>299</v>
-      </c>
-      <c r="E7" s="30" t="s">
-        <v>286</v>
-      </c>
-      <c r="F7" s="30" t="s">
-        <v>301</v>
-      </c>
       <c r="G7" s="35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H7" s="35" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="I7" s="21" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J7" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="18.5">
       <c r="A8" s="30" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="F8" s="30" t="s">
-        <v>302</v>
-      </c>
-      <c r="G8" s="43" t="s">
-        <v>77</v>
-      </c>
-      <c r="H8" s="43" t="s">
-        <v>253</v>
+        <v>298</v>
+      </c>
+      <c r="G8" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="H8" s="42" t="s">
+        <v>249</v>
       </c>
       <c r="I8" s="21" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="J8" s="22" t="s">
         <v>15</v>
@@ -1950,893 +1951,893 @@
     </row>
     <row r="9" spans="1:10" ht="15.5">
       <c r="A9" s="39" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B9" s="39" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C9" s="39" t="s">
-        <v>304</v>
+        <v>254</v>
       </c>
       <c r="D9" s="39" t="s">
         <v>81</v>
       </c>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H9" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I9" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="J9" s="23" t="s">
-        <v>16</v>
+        <v>131</v>
+      </c>
+      <c r="J9" s="24" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.5">
       <c r="A10" s="39" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B10" s="39" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C10" s="39" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D10" s="39" t="s">
-        <v>82</v>
-      </c>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
+        <v>86</v>
+      </c>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
       <c r="G10" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H10" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I10" s="21" t="s">
-        <v>133</v>
-      </c>
-      <c r="J10" s="23" t="s">
-        <v>17</v>
+        <v>136</v>
+      </c>
+      <c r="J10" s="22" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.5">
       <c r="A11" s="39" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B11" s="39" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C11" s="39" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D11" s="39" t="s">
-        <v>83</v>
-      </c>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
+        <v>87</v>
+      </c>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
       <c r="G11" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H11" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I11" s="21" t="s">
-        <v>134</v>
-      </c>
-      <c r="J11" s="24" t="s">
-        <v>19</v>
+        <v>137</v>
+      </c>
+      <c r="J11" s="22" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15.5">
       <c r="A12" s="39" t="s">
-        <v>189</v>
+        <v>219</v>
       </c>
       <c r="B12" s="39" t="s">
-        <v>275</v>
+        <v>240</v>
       </c>
       <c r="C12" s="39" t="s">
-        <v>260</v>
+        <v>46</v>
       </c>
       <c r="D12" s="39" t="s">
-        <v>84</v>
-      </c>
-      <c r="E12" s="40"/>
-      <c r="F12" s="40"/>
+        <v>111</v>
+      </c>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
       <c r="G12" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H12" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I12" s="21" t="s">
-        <v>135</v>
-      </c>
-      <c r="J12" s="22" t="s">
-        <v>0</v>
+        <v>166</v>
+      </c>
+      <c r="J12" s="23" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.5">
       <c r="A13" s="39" t="s">
-        <v>190</v>
+        <v>221</v>
       </c>
       <c r="B13" s="39" t="s">
-        <v>275</v>
+        <v>241</v>
       </c>
       <c r="C13" s="39" t="s">
-        <v>260</v>
+        <v>46</v>
       </c>
       <c r="D13" s="39" t="s">
-        <v>85</v>
-      </c>
-      <c r="E13" s="40"/>
-      <c r="F13" s="42"/>
+        <v>113</v>
+      </c>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
       <c r="G13" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H13" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I13" s="21" t="s">
-        <v>136</v>
-      </c>
-      <c r="J13" s="22" t="s">
-        <v>1</v>
+        <v>168</v>
+      </c>
+      <c r="J13" s="23" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.5">
       <c r="A14" s="39" t="s">
-        <v>191</v>
+        <v>223</v>
       </c>
       <c r="B14" s="39" t="s">
-        <v>275</v>
+        <v>241</v>
       </c>
       <c r="C14" s="39" t="s">
-        <v>260</v>
+        <v>46</v>
       </c>
       <c r="D14" s="39" t="s">
-        <v>86</v>
-      </c>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
+        <v>115</v>
+      </c>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
       <c r="G14" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H14" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I14" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="J14" s="22" t="s">
-        <v>2</v>
+        <v>170</v>
+      </c>
+      <c r="J14" s="23" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.5">
       <c r="A15" s="39" t="s">
-        <v>193</v>
+        <v>228</v>
       </c>
       <c r="B15" s="39" t="s">
-        <v>275</v>
+        <v>242</v>
       </c>
       <c r="C15" s="39" t="s">
-        <v>260</v>
+        <v>49</v>
       </c>
       <c r="D15" s="39" t="s">
-        <v>88</v>
-      </c>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
+        <v>120</v>
+      </c>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
       <c r="G15" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H15" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I15" s="21" t="s">
-        <v>139</v>
-      </c>
-      <c r="J15" s="22" t="s">
-        <v>4</v>
+        <v>175</v>
+      </c>
+      <c r="J15" s="23" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.5">
       <c r="A16" s="39" t="s">
-        <v>194</v>
+        <v>229</v>
       </c>
       <c r="B16" s="39" t="s">
-        <v>275</v>
+        <v>242</v>
       </c>
       <c r="C16" s="39" t="s">
-        <v>260</v>
+        <v>49</v>
       </c>
       <c r="D16" s="39" t="s">
-        <v>89</v>
-      </c>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
+        <v>121</v>
+      </c>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
       <c r="G16" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H16" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I16" s="21" t="s">
-        <v>140</v>
-      </c>
-      <c r="J16" s="22" t="s">
-        <v>5</v>
+        <v>176</v>
+      </c>
+      <c r="J16" s="23" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="15.5">
-      <c r="A17" s="39" t="s">
-        <v>223</v>
-      </c>
-      <c r="B17" s="39" t="s">
-        <v>244</v>
-      </c>
-      <c r="C17" s="39" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" s="39" t="s">
-        <v>113</v>
-      </c>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
+      <c r="A17" s="43" t="s">
+        <v>220</v>
+      </c>
+      <c r="B17" s="43" t="s">
+        <v>240</v>
+      </c>
+      <c r="C17" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="43" t="s">
+        <v>112</v>
+      </c>
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
       <c r="G17" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H17" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I17" s="21" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J17" s="23" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="15.5">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="43" t="s">
+        <v>230</v>
+      </c>
+      <c r="B18" s="43" t="s">
+        <v>242</v>
+      </c>
+      <c r="C18" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="43" t="s">
+        <v>122</v>
+      </c>
+      <c r="E18" s="44"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="H18" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="I18" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="J18" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="15.5">
+      <c r="A19" s="43" t="s">
+        <v>231</v>
+      </c>
+      <c r="B19" s="43" t="s">
+        <v>243</v>
+      </c>
+      <c r="C19" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="43" t="s">
+        <v>123</v>
+      </c>
+      <c r="E19" s="44"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="H19" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="I19" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="J19" s="23" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="15.5">
+      <c r="A20" s="43" t="s">
+        <v>233</v>
+      </c>
+      <c r="B20" s="43" t="s">
+        <v>243</v>
+      </c>
+      <c r="C20" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="43" t="s">
+        <v>125</v>
+      </c>
+      <c r="E20" s="44"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="H20" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="I20" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="J20" s="23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="15.5">
+      <c r="A21" s="43" t="s">
+        <v>181</v>
+      </c>
+      <c r="B21" s="43" t="s">
+        <v>271</v>
+      </c>
+      <c r="C21" s="43" t="s">
+        <v>255</v>
+      </c>
+      <c r="D21" s="43" t="s">
+        <v>78</v>
+      </c>
+      <c r="E21" s="44"/>
+      <c r="F21" s="44"/>
+      <c r="G21" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="H21" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="I21" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="J21" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="15.5">
+      <c r="A22" s="43" t="s">
+        <v>185</v>
+      </c>
+      <c r="B22" s="43" t="s">
+        <v>271</v>
+      </c>
+      <c r="C22" s="43" t="s">
+        <v>256</v>
+      </c>
+      <c r="D22" s="43" t="s">
+        <v>82</v>
+      </c>
+      <c r="E22" s="45"/>
+      <c r="F22" s="45"/>
+      <c r="G22" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="H22" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="I22" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="J22" s="22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="15.5">
+      <c r="A23" s="43" t="s">
+        <v>186</v>
+      </c>
+      <c r="B23" s="43" t="s">
+        <v>271</v>
+      </c>
+      <c r="C23" s="43" t="s">
+        <v>256</v>
+      </c>
+      <c r="D23" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="E23" s="45"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="H23" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="I23" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="J23" s="22" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="15.5">
+      <c r="A24" s="43" t="s">
+        <v>183</v>
+      </c>
+      <c r="B24" s="43" t="s">
+        <v>271</v>
+      </c>
+      <c r="C24" s="43" t="s">
+        <v>299</v>
+      </c>
+      <c r="D24" s="43" t="s">
+        <v>80</v>
+      </c>
+      <c r="E24" s="44"/>
+      <c r="F24" s="44"/>
+      <c r="G24" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="H24" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="I24" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="J24" s="23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="15.5">
+      <c r="A25" s="43" t="s">
+        <v>187</v>
+      </c>
+      <c r="B25" s="43" t="s">
+        <v>271</v>
+      </c>
+      <c r="C25" s="43" t="s">
+        <v>256</v>
+      </c>
+      <c r="D25" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="E25" s="45"/>
+      <c r="F25" s="45"/>
+      <c r="G25" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="H25" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="I25" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="J25" s="22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="15.5">
+      <c r="A26" s="43" t="s">
         <v>224</v>
       </c>
-      <c r="B18" s="39" t="s">
-        <v>244</v>
-      </c>
-      <c r="C18" s="39" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" s="39" t="s">
-        <v>114</v>
-      </c>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="35" t="s">
-        <v>73</v>
-      </c>
-      <c r="H18" s="35" t="s">
-        <v>73</v>
-      </c>
-      <c r="I18" s="21" t="s">
-        <v>170</v>
-      </c>
-      <c r="J18" s="23" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="15.5">
-      <c r="A19" s="39" t="s">
+      <c r="B26" s="43" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="D26" s="43" t="s">
+        <v>116</v>
+      </c>
+      <c r="E26" s="44"/>
+      <c r="F26" s="44"/>
+      <c r="G26" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="H26" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="I26" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="J26" s="23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="15.5">
+      <c r="A27" s="43" t="s">
         <v>225</v>
       </c>
-      <c r="B19" s="39" t="s">
-        <v>245</v>
-      </c>
-      <c r="C19" s="39" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19" s="39" t="s">
-        <v>115</v>
-      </c>
-      <c r="E19" s="41"/>
-      <c r="F19" s="41"/>
-      <c r="G19" s="35" t="s">
-        <v>73</v>
-      </c>
-      <c r="H19" s="35" t="s">
-        <v>73</v>
-      </c>
-      <c r="I19" s="21" t="s">
-        <v>171</v>
-      </c>
-      <c r="J19" s="23" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="15.5">
-      <c r="A20" s="39" t="s">
+      <c r="B27" s="43" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" s="43" t="s">
+        <v>117</v>
+      </c>
+      <c r="E27" s="44"/>
+      <c r="F27" s="44"/>
+      <c r="G27" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="H27" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="I27" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="J27" s="23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="15.5">
+      <c r="A28" s="43" t="s">
+        <v>226</v>
+      </c>
+      <c r="B28" s="43" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28" s="43" t="s">
+        <v>118</v>
+      </c>
+      <c r="E28" s="44"/>
+      <c r="F28" s="44"/>
+      <c r="G28" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="H28" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="I28" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="J28" s="23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="15.5">
+      <c r="A29" s="43" t="s">
         <v>227</v>
       </c>
-      <c r="B20" s="39" t="s">
-        <v>245</v>
-      </c>
-      <c r="C20" s="39" t="s">
-        <v>47</v>
-      </c>
-      <c r="D20" s="39" t="s">
-        <v>117</v>
-      </c>
-      <c r="E20" s="41"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="35" t="s">
-        <v>73</v>
-      </c>
-      <c r="H20" s="35" t="s">
-        <v>73</v>
-      </c>
-      <c r="I20" s="21" t="s">
-        <v>173</v>
-      </c>
-      <c r="J20" s="23" t="s">
+      <c r="B29" s="43" t="s">
+        <v>242</v>
+      </c>
+      <c r="C29" s="43" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" ht="15.5">
-      <c r="A21" s="39" t="s">
-        <v>228</v>
-      </c>
-      <c r="B21" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="39" t="s">
-        <v>47</v>
-      </c>
-      <c r="D21" s="39" t="s">
-        <v>118</v>
-      </c>
-      <c r="E21" s="41"/>
-      <c r="F21" s="41"/>
-      <c r="G21" s="35" t="s">
-        <v>73</v>
-      </c>
-      <c r="H21" s="35" t="s">
-        <v>73</v>
-      </c>
-      <c r="I21" s="21" t="s">
+      <c r="D29" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="H29" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="I29" s="21" t="s">
         <v>174</v>
       </c>
-      <c r="J21" s="23" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="15.5">
-      <c r="A22" s="39" t="s">
-        <v>229</v>
-      </c>
-      <c r="B22" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="C22" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="D22" s="39" t="s">
-        <v>119</v>
-      </c>
-      <c r="E22" s="41"/>
-      <c r="F22" s="41"/>
-      <c r="G22" s="35" t="s">
-        <v>73</v>
-      </c>
-      <c r="H22" s="35" t="s">
-        <v>73</v>
-      </c>
-      <c r="I22" s="21" t="s">
-        <v>175</v>
-      </c>
-      <c r="J22" s="23" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="15.5">
-      <c r="A23" s="39" t="s">
-        <v>230</v>
-      </c>
-      <c r="B23" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="C23" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="D23" s="39" t="s">
-        <v>120</v>
-      </c>
-      <c r="E23" s="41"/>
-      <c r="F23" s="41"/>
-      <c r="G23" s="35" t="s">
-        <v>73</v>
-      </c>
-      <c r="H23" s="35" t="s">
-        <v>73</v>
-      </c>
-      <c r="I23" s="21" t="s">
-        <v>176</v>
-      </c>
-      <c r="J23" s="23" t="s">
+      <c r="J29" s="23" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15.5">
-      <c r="A24" s="39" t="s">
-        <v>231</v>
-      </c>
-      <c r="B24" s="39" t="s">
-        <v>246</v>
-      </c>
-      <c r="C24" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="D24" s="39" t="s">
-        <v>121</v>
-      </c>
-      <c r="E24" s="41"/>
-      <c r="F24" s="41"/>
-      <c r="G24" s="35" t="s">
-        <v>73</v>
-      </c>
-      <c r="H24" s="35" t="s">
-        <v>73</v>
-      </c>
-      <c r="I24" s="21" t="s">
-        <v>177</v>
-      </c>
-      <c r="J24" s="23" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="15.5">
-      <c r="A25" s="39" t="s">
-        <v>232</v>
-      </c>
-      <c r="B25" s="39" t="s">
-        <v>246</v>
-      </c>
-      <c r="C25" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="D25" s="39" t="s">
-        <v>122</v>
-      </c>
-      <c r="E25" s="41"/>
-      <c r="F25" s="41"/>
-      <c r="G25" s="35" t="s">
-        <v>73</v>
-      </c>
-      <c r="H25" s="35" t="s">
-        <v>73</v>
-      </c>
-      <c r="I25" s="21" t="s">
-        <v>178</v>
-      </c>
-      <c r="J25" s="23" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="15.5">
-      <c r="A26" s="39" t="s">
-        <v>233</v>
-      </c>
-      <c r="B26" s="39" t="s">
-        <v>246</v>
-      </c>
-      <c r="C26" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="D26" s="39" t="s">
-        <v>123</v>
-      </c>
-      <c r="E26" s="41"/>
-      <c r="F26" s="41"/>
-      <c r="G26" s="35" t="s">
-        <v>73</v>
-      </c>
-      <c r="H26" s="35" t="s">
-        <v>73</v>
-      </c>
-      <c r="I26" s="21" t="s">
-        <v>179</v>
-      </c>
-      <c r="J26" s="23" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="15.5">
-      <c r="A27" s="39" t="s">
-        <v>234</v>
-      </c>
-      <c r="B27" s="39" t="s">
-        <v>246</v>
-      </c>
-      <c r="C27" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="D27" s="39" t="s">
-        <v>124</v>
-      </c>
-      <c r="E27" s="41"/>
-      <c r="F27" s="41"/>
-      <c r="G27" s="35" t="s">
-        <v>73</v>
-      </c>
-      <c r="H27" s="35" t="s">
-        <v>73</v>
-      </c>
-      <c r="I27" s="21" t="s">
-        <v>180</v>
-      </c>
-      <c r="J27" s="23" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="15.5">
-      <c r="A28" s="39" t="s">
-        <v>235</v>
-      </c>
-      <c r="B28" s="39" t="s">
-        <v>247</v>
-      </c>
-      <c r="C28" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="D28" s="39" t="s">
-        <v>125</v>
-      </c>
-      <c r="E28" s="41"/>
-      <c r="F28" s="41"/>
-      <c r="G28" s="35" t="s">
-        <v>73</v>
-      </c>
-      <c r="H28" s="35" t="s">
-        <v>73</v>
-      </c>
-      <c r="I28" s="21" t="s">
-        <v>181</v>
-      </c>
-      <c r="J28" s="23" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="15.5">
-      <c r="A29" s="39" t="s">
-        <v>237</v>
-      </c>
-      <c r="B29" s="39" t="s">
-        <v>247</v>
-      </c>
-      <c r="C29" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="D29" s="39" t="s">
-        <v>127</v>
-      </c>
-      <c r="E29" s="41"/>
-      <c r="F29" s="41"/>
-      <c r="G29" s="35" t="s">
-        <v>73</v>
-      </c>
-      <c r="H29" s="35" t="s">
-        <v>73</v>
-      </c>
-      <c r="I29" s="21" t="s">
-        <v>182</v>
-      </c>
-      <c r="J29" s="23" t="s">
-        <v>59</v>
-      </c>
-    </row>
     <row r="30" spans="1:10" ht="15.5">
-      <c r="A30" s="39" t="s">
-        <v>184</v>
-      </c>
-      <c r="B30" s="39" t="s">
-        <v>275</v>
-      </c>
-      <c r="C30" s="39" t="s">
-        <v>259</v>
-      </c>
-      <c r="D30" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="E30" s="41"/>
-      <c r="F30" s="41"/>
+      <c r="A30" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
       <c r="G30" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H30" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I30" s="21" t="s">
-        <v>130</v>
-      </c>
-      <c r="J30" s="16" t="s">
-        <v>14</v>
+        <v>138</v>
+      </c>
+      <c r="J30" s="22" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="15.5">
       <c r="A31" s="9" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
       <c r="G31" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H31" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I31" s="21" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="J31" s="22" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="15.5">
       <c r="A32" s="9" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E32" s="10"/>
       <c r="F32" s="10"/>
       <c r="G32" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H32" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I32" s="21" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="J32" s="22" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="15.5">
       <c r="A33" s="9" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E33" s="10"/>
       <c r="F33" s="10"/>
       <c r="G33" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H33" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I33" s="21" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J33" s="22" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="15.5">
       <c r="A34" s="9" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E34" s="10"/>
       <c r="F34" s="10"/>
       <c r="G34" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H34" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I34" s="21" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="J34" s="22" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="15.5">
       <c r="A35" s="9" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>275</v>
+        <v>236</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="E35" s="10"/>
-      <c r="F35" s="10"/>
+        <v>93</v>
+      </c>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
       <c r="G35" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H35" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I35" s="21" t="s">
-        <v>145</v>
-      </c>
-      <c r="J35" s="22" t="s">
-        <v>10</v>
+        <v>143</v>
+      </c>
+      <c r="J35" s="23" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="15.5">
       <c r="A36" s="9" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
+        <v>94</v>
+      </c>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
       <c r="G36" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H36" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I36" s="21" t="s">
-        <v>146</v>
-      </c>
-      <c r="J36" s="23" t="s">
-        <v>284</v>
+        <v>144</v>
+      </c>
+      <c r="J36" s="22" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="15.5">
       <c r="A37" s="9" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E37" s="12"/>
       <c r="F37" s="12"/>
       <c r="G37" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H37" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I37" s="21" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="J37" s="22" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="15.5">
       <c r="A38" s="9" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
+        <v>13</v>
+      </c>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
       <c r="G38" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H38" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I38" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="J38" s="22" t="s">
-        <v>12</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="J38" s="24"/>
     </row>
     <row r="39" spans="1:10" ht="15.5">
       <c r="A39" s="9" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
+        <v>96</v>
+      </c>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
       <c r="G39" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H39" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I39" s="21" t="s">
-        <v>149</v>
-      </c>
-      <c r="J39" s="24"/>
+        <v>147</v>
+      </c>
+      <c r="J39" s="23" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="40" spans="1:10" ht="15.5">
       <c r="A40" s="9" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E40" s="11"/>
       <c r="F40" s="11"/>
       <c r="G40" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H40" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I40" s="21" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J40" s="23" t="s">
         <v>20</v>
@@ -2844,27 +2845,27 @@
     </row>
     <row r="41" spans="1:10" ht="15.5">
       <c r="A41" s="9" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E41" s="11"/>
       <c r="F41" s="11"/>
       <c r="G41" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H41" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I41" s="21" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="J41" s="23" t="s">
         <v>21</v>
@@ -2872,55 +2873,55 @@
     </row>
     <row r="42" spans="1:10" ht="15.5">
       <c r="A42" s="9" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>100</v>
+        <v>22</v>
       </c>
       <c r="E42" s="11"/>
       <c r="F42" s="11"/>
       <c r="G42" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H42" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I42" s="21" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="J42" s="23" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="15.5">
       <c r="A43" s="9" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>23</v>
+        <v>99</v>
       </c>
       <c r="E43" s="11"/>
       <c r="F43" s="11"/>
       <c r="G43" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H43" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I43" s="21" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="J43" s="23" t="s">
         <v>24</v>
@@ -2928,27 +2929,27 @@
     </row>
     <row r="44" spans="1:10" ht="15.5">
       <c r="A44" s="9" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E44" s="11"/>
       <c r="F44" s="11"/>
       <c r="G44" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H44" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I44" s="21" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="J44" s="23" t="s">
         <v>25</v>
@@ -2956,27 +2957,27 @@
     </row>
     <row r="45" spans="1:10" ht="15.5">
       <c r="A45" s="9" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E45" s="11"/>
       <c r="F45" s="11"/>
       <c r="G45" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H45" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I45" s="21" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="J45" s="23" t="s">
         <v>26</v>
@@ -2984,27 +2985,27 @@
     </row>
     <row r="46" spans="1:10" ht="15.5">
       <c r="A46" s="9" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E46" s="11"/>
       <c r="F46" s="11"/>
       <c r="G46" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H46" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I46" s="21" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="J46" s="23" t="s">
         <v>27</v>
@@ -3012,27 +3013,27 @@
     </row>
     <row r="47" spans="1:10" ht="15.5">
       <c r="A47" s="9" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E47" s="11"/>
       <c r="F47" s="11"/>
       <c r="G47" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H47" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I47" s="21" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J47" s="23" t="s">
         <v>28</v>
@@ -3040,27 +3041,27 @@
     </row>
     <row r="48" spans="1:10" ht="15.5">
       <c r="A48" s="9" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E48" s="11"/>
       <c r="F48" s="11"/>
       <c r="G48" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H48" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I48" s="21" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J48" s="23" t="s">
         <v>29</v>
@@ -3068,55 +3069,55 @@
     </row>
     <row r="49" spans="1:10" ht="15.5">
       <c r="A49" s="9" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>106</v>
+        <v>30</v>
       </c>
       <c r="E49" s="11"/>
       <c r="F49" s="11"/>
       <c r="G49" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H49" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I49" s="21" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J49" s="23" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="15.5">
       <c r="A50" s="9" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>31</v>
+        <v>105</v>
       </c>
       <c r="E50" s="11"/>
       <c r="F50" s="11"/>
       <c r="G50" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H50" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I50" s="21" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="J50" s="23" t="s">
         <v>32</v>
@@ -3124,27 +3125,27 @@
     </row>
     <row r="51" spans="1:10" ht="15.5">
       <c r="A51" s="9" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E51" s="11"/>
       <c r="F51" s="11"/>
       <c r="G51" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H51" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I51" s="21" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J51" s="23" t="s">
         <v>33</v>
@@ -3152,261 +3153,233 @@
     </row>
     <row r="52" spans="1:10" ht="15.5">
       <c r="A52" s="9" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>108</v>
+        <v>34</v>
       </c>
       <c r="E52" s="11"/>
       <c r="F52" s="11"/>
       <c r="G52" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H52" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I52" s="21" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="J52" s="23" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="15.5">
       <c r="A53" s="9" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E53" s="11"/>
       <c r="F53" s="11"/>
       <c r="G53" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H53" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I53" s="21" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="J53" s="23" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="15.5">
       <c r="A54" s="9" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E54" s="11"/>
-      <c r="F54" s="11"/>
+        <v>107</v>
+      </c>
+      <c r="E54" s="12"/>
+      <c r="F54" s="12"/>
       <c r="G54" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H54" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I54" s="21" t="s">
-        <v>164</v>
-      </c>
-      <c r="J54" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="J54" s="22" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="15.5">
       <c r="A55" s="9" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="E55" s="12"/>
-      <c r="F55" s="12"/>
+        <v>108</v>
+      </c>
+      <c r="E55" s="11"/>
+      <c r="F55" s="11"/>
       <c r="G55" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H55" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I55" s="21" t="s">
-        <v>165</v>
-      </c>
-      <c r="J55" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="J55" s="23" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="15.5">
       <c r="A56" s="9" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="E56" s="11"/>
-      <c r="F56" s="11"/>
+        <v>109</v>
+      </c>
+      <c r="E56" s="12"/>
+      <c r="F56" s="12"/>
       <c r="G56" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H56" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I56" s="21" t="s">
-        <v>166</v>
-      </c>
-      <c r="J56" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="J56" s="22" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="15.5">
       <c r="A57" s="9" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="E57" s="12"/>
-      <c r="F57" s="12"/>
+        <v>110</v>
+      </c>
+      <c r="E57" s="11"/>
+      <c r="F57" s="11"/>
       <c r="G57" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H57" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I57" s="21" t="s">
-        <v>167</v>
-      </c>
-      <c r="J57" s="22" t="s">
-        <v>41</v>
+        <v>165</v>
+      </c>
+      <c r="J57" s="23" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="15.5">
-      <c r="A58" s="9" t="s">
+      <c r="A58" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="B58" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="C58" s="9" t="s">
-        <v>261</v>
-      </c>
-      <c r="D58" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="E58" s="11"/>
-      <c r="F58" s="11"/>
+      <c r="B58" s="36" t="s">
+        <v>241</v>
+      </c>
+      <c r="C58" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="D58" s="36" t="s">
+        <v>114</v>
+      </c>
+      <c r="E58" s="37"/>
+      <c r="F58" s="37"/>
       <c r="G58" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H58" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I58" s="21" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="J58" s="23" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="15.5">
       <c r="A59" s="36" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="B59" s="36" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C59" s="36" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D59" s="36" t="s">
-        <v>116</v>
-      </c>
-      <c r="E59" s="37"/>
-      <c r="F59" s="37"/>
+        <v>124</v>
+      </c>
+      <c r="E59" s="38"/>
+      <c r="F59" s="38"/>
       <c r="G59" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H59" s="35" t="s">
-        <v>73</v>
-      </c>
-      <c r="I59" s="21" t="s">
-        <v>172</v>
-      </c>
-      <c r="J59" s="23" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" ht="15.5">
-      <c r="A60" s="36" t="s">
-        <v>236</v>
-      </c>
-      <c r="B60" s="36" t="s">
-        <v>247</v>
-      </c>
-      <c r="C60" s="36" t="s">
-        <v>50</v>
-      </c>
-      <c r="D60" s="36" t="s">
-        <v>126</v>
-      </c>
-      <c r="E60" s="38"/>
-      <c r="F60" s="38"/>
-      <c r="G60" s="35" t="s">
-        <v>73</v>
-      </c>
-      <c r="H60" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G2:J5 I6:J59 G6:H60">
+  <conditionalFormatting sqref="I15:J58 G15:H59 G2:J14 G17:J17">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"undefined"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H60 H2:J59" xr:uid="{E4DF7DBE-233E-4CAB-B72C-331851F0FA04}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H59 H2:J12 H13:J58" xr:uid="{E4DF7DBE-233E-4CAB-B72C-331851F0FA04}">
       <formula1>"undefined,yes,no"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G60" xr:uid="{27BB500F-5D24-420A-87D6-C1F235E36EA2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G12 G13:G59" xr:uid="{27BB500F-5D24-420A-87D6-C1F235E36EA2}">
       <formula1>"undefined,check,info"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3420,7 +3393,7 @@
   <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3443,248 +3416,248 @@
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B2" t="s">
+        <v>261</v>
+      </c>
+      <c r="C2" t="s">
+        <v>262</v>
+      </c>
+      <c r="D2" t="s">
+        <v>255</v>
+      </c>
+      <c r="E2" t="s">
+        <v>263</v>
+      </c>
+      <c r="F2" t="s">
+        <v>248</v>
+      </c>
+      <c r="G2" t="s">
+        <v>248</v>
+      </c>
+      <c r="H2" t="s">
+        <v>248</v>
+      </c>
+      <c r="I2" t="s">
+        <v>249</v>
+      </c>
+      <c r="J2" t="s">
+        <v>249</v>
+      </c>
+      <c r="K2" t="s">
         <v>264</v>
-      </c>
-      <c r="B2" t="s">
-        <v>265</v>
-      </c>
-      <c r="C2" t="s">
-        <v>266</v>
-      </c>
-      <c r="D2" t="s">
-        <v>259</v>
-      </c>
-      <c r="E2" t="s">
-        <v>267</v>
-      </c>
-      <c r="F2" t="s">
-        <v>252</v>
-      </c>
-      <c r="G2" t="s">
-        <v>252</v>
-      </c>
-      <c r="H2" t="s">
-        <v>252</v>
-      </c>
-      <c r="I2" t="s">
-        <v>253</v>
-      </c>
-      <c r="J2" t="s">
-        <v>253</v>
-      </c>
-      <c r="K2" t="s">
-        <v>268</v>
       </c>
       <c r="N2" s="1"/>
       <c r="Q2" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" spans="1:17">
       <c r="A3" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="B3" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="C3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="D3" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F3" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="G3" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="H3" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="I3" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="J3" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="L3" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="M3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="Q3" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B4" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="C4" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="D4" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="E4" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="F4" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="G4" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="H4" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="I4" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="J4" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="N4" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="O4">
         <v>123</v>
       </c>
       <c r="Q4" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="5" spans="1:17">
       <c r="A5" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="B5" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C5" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="D5" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="E5" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="F5" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="G5" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="H5" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="I5" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="J5" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="N5" s="1"/>
       <c r="Q5" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="6" spans="1:17">
       <c r="A6" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="B6" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C6" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="D6" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="E6" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="F6" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="G6" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="I6" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="J6" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="O6" s="1"/>
       <c r="Q6" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="8" spans="1:17">

</xml_diff>